<commit_message>
ADD:Agregar comentarios al diccionario de datos
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de sistema/Base de datos/Diccionario de datos BD.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de sistema/Base de datos/Diccionario de datos BD.xlsx
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="383">
   <si>
     <t>Diccionario de datos BD</t>
   </si>
@@ -727,15 +727,15 @@
     <t>date</t>
   </si>
   <si>
+    <t>2B383476-AC5D-1802-D02D-FF4D722B6616</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>81011408-6140-186E-5869-1329F0D44FFA</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>2B383476-AC5D-1802-D02D-FF4D722B6616</t>
-  </si>
-  <si>
     <t>0DC8528D-621E-B3E6-D588-8692D6E45ECE</t>
   </si>
   <si>
@@ -754,42 +754,42 @@
     <t>fixedCost</t>
   </si>
   <si>
+    <t>5257B76A-61F8-1740-CF51-4561C8C5B6CD</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>FD482B8E-FAC4-14B8-B6F7-4BB4493553D6</t>
+  </si>
+  <si>
+    <t>C66B576B-F4C3-B565-CBCC-2F9C07762CEB</t>
+  </si>
+  <si>
+    <t>18A15F6C-C5AC-809C-69A3-14404A8C4E90</t>
+  </si>
+  <si>
+    <t>0DED2D0A-5259-C377-320D-508BC6692377</t>
+  </si>
+  <si>
+    <t>46638D63-590B-1E3B-DBE5-F3F7DEA8BE87</t>
+  </si>
+  <si>
     <t>BF7E657D-D05A-0499-FF45-39AE4BBD13D2</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>5257B76A-61F8-1740-CF51-4561C8C5B6CD</t>
-  </si>
-  <si>
-    <t>46638D63-590B-1E3B-DBE5-F3F7DEA8BE87</t>
-  </si>
-  <si>
-    <t>FD482B8E-FAC4-14B8-B6F7-4BB4493553D6</t>
+    <t>E562EC6C-79B5-BB43-A61E-0BDCE6F58C77</t>
+  </si>
+  <si>
+    <t>C6B9DCF9-EBFB-8590-7CB3-4536F9387A30</t>
+  </si>
+  <si>
+    <t>88182613-8C6B-8237-4F2B-E8615A23F3CF</t>
   </si>
   <si>
     <t>DED107D2-07E2-FE6A-19B3-970E7C3D9AC5</t>
   </si>
   <si>
-    <t>C66B576B-F4C3-B565-CBCC-2F9C07762CEB</t>
-  </si>
-  <si>
-    <t>88182613-8C6B-8237-4F2B-E8615A23F3CF</t>
-  </si>
-  <si>
-    <t>0DED2D0A-5259-C377-320D-508BC6692377</t>
-  </si>
-  <si>
-    <t>C6B9DCF9-EBFB-8590-7CB3-4536F9387A30</t>
-  </si>
-  <si>
-    <t>18A15F6C-C5AC-809C-69A3-14404A8C4E90</t>
-  </si>
-  <si>
-    <t>E562EC6C-79B5-BB43-A61E-0BDCE6F58C77</t>
-  </si>
-  <si>
     <t>7961CC4F-BA66-2228-A932-0B0346F7A562</t>
   </si>
   <si>
@@ -883,21 +883,21 @@
     <t>4958C6A9-8928-AFF9-F8B9-E4368BDF72B4</t>
   </si>
   <si>
+    <t>FADC9424-B13F-6201-4225-C82C31C6B6C7</t>
+  </si>
+  <si>
     <t>F0C220D1-1997-F6A7-56B2-19A7C44C6152</t>
   </si>
   <si>
+    <t>22BEF716-1B55-B0BA-1EFD-B33AA7BF463A</t>
+  </si>
+  <si>
+    <t>525758B3-8BF8-B3F4-269D-7E269B8FB8D6</t>
+  </si>
+  <si>
     <t>2CA22C0F-3E70-79E3-4CC1-4D8A18C741B5</t>
   </si>
   <si>
-    <t>FADC9424-B13F-6201-4225-C82C31C6B6C7</t>
-  </si>
-  <si>
-    <t>525758B3-8BF8-B3F4-269D-7E269B8FB8D6</t>
-  </si>
-  <si>
-    <t>22BEF716-1B55-B0BA-1EFD-B33AA7BF463A</t>
-  </si>
-  <si>
     <t>1B3869AC-9231-7FC5-BD2B-AF1B3A58E1BC</t>
   </si>
   <si>
@@ -1615,6 +1615,15 @@
     <t>VARCHAR2 (10)</t>
   </si>
   <si>
+    <t xml:space="preserve">Ejemplo:
+BT1
+BT2
+BT1-T3
+AT2
+AT3
+</t>
+  </si>
+  <si>
     <t>ChargeType.id</t>
   </si>
   <si>
@@ -1625,6 +1634,15 @@
   </si>
   <si>
     <t>NUMBER (20,2)</t>
+  </si>
+  <si>
+    <t>Costo Fijo</t>
+  </si>
+  <si>
+    <t>Tipo de tarifa</t>
+  </si>
+  <si>
+    <t>Costo Variable</t>
   </si>
   <si>
     <t>Contract.id</t>
@@ -2380,7 +2398,7 @@
         <v>322</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>322</v>
+        <v>354</v>
       </c>
     </row>
     <row r="38" ht="18.0" customHeight="true">
@@ -2419,7 +2437,7 @@
         <v>341</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>322</v>
@@ -2524,7 +2542,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>334</v>
@@ -2578,7 +2596,7 @@
         <v>341</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>322</v>
@@ -2675,7 +2693,7 @@
         <v>322</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
     </row>
     <row r="61" ht="18.0" customHeight="true">
@@ -2721,7 +2739,7 @@
         <v>322</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>322</v>
+        <v>360</v>
       </c>
     </row>
     <row r="63" ht="18.0" customHeight="true">
@@ -2752,7 +2770,7 @@
         <v>100</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>334</v>
@@ -2790,7 +2808,7 @@
         <v>322</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" ht="18.0" customHeight="true">
@@ -2829,7 +2847,7 @@
         <v>341</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>322</v>
@@ -3008,7 +3026,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>334</v>
@@ -3062,7 +3080,7 @@
         <v>341</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>322</v>
@@ -3167,7 +3185,7 @@
         <v>108</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>334</v>
@@ -3190,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>334</v>
@@ -3213,7 +3231,7 @@
         <v>124</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>334</v>
@@ -3267,7 +3285,7 @@
         <v>341</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>322</v>
@@ -3284,10 +3302,10 @@
         <v>178</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>322</v>
@@ -3392,7 +3410,7 @@
         <v>3</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>334</v>
@@ -3446,7 +3464,7 @@
         <v>341</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="F118" s="6" t="s">
         <v>322</v>
@@ -3551,7 +3569,7 @@
         <v>3</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>334</v>
@@ -3605,7 +3623,7 @@
         <v>341</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>322</v>
@@ -3648,7 +3666,7 @@
         <v>322</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F134" s="6" t="s">
         <v>322</v>
@@ -3687,7 +3705,7 @@
         <v>51</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>336</v>
@@ -3710,7 +3728,7 @@
         <v>57</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D139" s="8" t="s">
         <v>336</v>
@@ -3779,7 +3797,7 @@
         <v>98</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>336</v>
@@ -3802,7 +3820,7 @@
         <v>120</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D143" s="8" t="s">
         <v>336</v>
@@ -3856,7 +3874,7 @@
         <v>341</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F148" s="6" t="s">
         <v>322</v>
@@ -3989,7 +4007,7 @@
         <v>53</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D160" s="8" t="s">
         <v>336</v>
@@ -4012,7 +4030,7 @@
         <v>62</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D161" s="8" t="s">
         <v>334</v>
@@ -4035,7 +4053,7 @@
         <v>64</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D162" s="8" t="s">
         <v>336</v>
@@ -4127,7 +4145,7 @@
         <v>104</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D166" s="8" t="s">
         <v>336</v>
@@ -4150,7 +4168,7 @@
         <v>106</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D167" s="8" t="s">
         <v>336</v>
@@ -4173,7 +4191,7 @@
         <v>116</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D168" s="8" t="s">
         <v>336</v>
@@ -4196,7 +4214,7 @@
         <v>118</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D169" s="8" t="s">
         <v>334</v>
@@ -4219,7 +4237,7 @@
         <v>122</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D170" s="8" t="s">
         <v>336</v>
@@ -4273,7 +4291,7 @@
         <v>341</v>
       </c>
       <c r="E175" s="8" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F175" s="6" t="s">
         <v>322</v>
@@ -4452,7 +4470,7 @@
         <v>49</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D189" s="8" t="s">
         <v>336</v>
@@ -4475,7 +4493,7 @@
         <v>55</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D190" s="8" t="s">
         <v>334</v>
@@ -4498,7 +4516,7 @@
         <v>59</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D191" s="8" t="s">
         <v>336</v>
@@ -4567,7 +4585,7 @@
         <v>102</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D194" s="8" t="s">
         <v>334</v>
@@ -4590,7 +4608,7 @@
         <v>126</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D195" s="8" t="s">
         <v>334</v>
@@ -4644,7 +4662,7 @@
         <v>341</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="F200" s="6" t="s">
         <v>322</v>

</xml_diff>

<commit_message>
Cambiar nombre user a diagramas
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de sistema/Base de datos/Diccionario de datos BD.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de sistema/Base de datos/Diccionario de datos BD.xlsx
@@ -110,370 +110,370 @@
     </comment>
     <comment ref="A30" authorId="0">
       <text>
+        <t>ObjectID:9EB277BE-7029-BA3A-7ED2-D3038A5BB0F7;
+Class:oracle.dbtools.crest.model.design.relational.Table</t>
+      </text>
+    </comment>
+    <comment ref="B34" authorId="0">
+      <text>
+        <t>ObjectID:0A748269-11F0-6F0A-4667-79981867EE71;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="0">
+      <text>
+        <t>ObjectID:0DC8528D-621E-B3E6-D588-8692D6E45ECE;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B36" authorId="0">
+      <text>
+        <t>ObjectID:BD88747F-A567-E695-8FB1-F158C888E4A5;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B37" authorId="0">
+      <text>
+        <t>ObjectID:C6B9DCF9-EBFB-8590-7CB3-4536F9387A30;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0">
+      <text>
+        <t>ObjectID:7961CC4F-BA66-2228-A932-0B0346F7A562;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0">
+      <text>
+        <t>ObjectID:116A239F-1C67-FC1B-6815-35D5ACAE992B;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0">
+      <text>
+        <t>ObjectID:D4892A06-5DB8-541D-0CE1-87349B9F7CF4;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B41" authorId="0">
+      <text>
+        <t>ObjectID:BFBDF889-A7E4-DCFD-EBC4-7B96A816B970;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B42" authorId="0">
+      <text>
+        <t>ObjectID:1B3869AC-9231-7FC5-BD2B-AF1B3A58E1BC;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0">
+      <text>
+        <t>ObjectID:506CC65D-B1AB-F31A-4BA9-517671DDF7B6;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <t>ObjectID:EFBBC641-A321-85C6-19C5-7484C997CEB6;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="0">
+      <text>
+        <t>ObjectID:DB34C21D-3EE5-7339-632A-053443C65A1D;
+Class:oracle.dbtools.crest.model.design.relational.Index</t>
+      </text>
+    </comment>
+    <comment ref="B54" authorId="0">
+      <text>
+        <t>ObjectID:5672E553-2046-F443-A1CF-5056EFCC6128;
+Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
+      </text>
+    </comment>
+    <comment ref="B55" authorId="0">
+      <text>
+        <t>ObjectID:E465E2CF-3E8A-BC03-97AD-612D80B1ED1A;
+Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
+      </text>
+    </comment>
+    <comment ref="A58" authorId="0">
+      <text>
         <t>ObjectID:18144285-2A12-39D4-D8F8-0A3A21C806E9;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B62" authorId="0">
       <text>
         <t>ObjectID:5257B76A-61F8-1740-CF51-4561C8C5B6CD;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B35" authorId="0">
+    <comment ref="B63" authorId="0">
       <text>
         <t>ObjectID:4958C6A9-8928-AFF9-F8B9-E4368BDF72B4;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B40" authorId="0">
+    <comment ref="B68" authorId="0">
       <text>
         <t>ObjectID:A3A2543F-CEE5-46DD-9744-09F43056D2BD;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="A43" authorId="0">
+    <comment ref="A71" authorId="0">
       <text>
         <t>ObjectID:6CD2FFF6-9693-F671-C30B-FC18055CE5C9;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B47" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <t>ObjectID:46638D63-590B-1E3B-DBE5-F3F7DEA8BE87;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B48" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <t>ObjectID:F0C220D1-1997-F6A7-56B2-19A7C44C6152;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B53" authorId="0">
+    <comment ref="B81" authorId="0">
       <text>
         <t>ObjectID:22C00C2E-977B-6A07-6FDB-8E01B138AD3B;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="A56" authorId="0">
+    <comment ref="A84" authorId="0">
       <text>
         <t>ObjectID:3C6E51DE-D959-2082-62D4-45B31B87D6BE;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B60" authorId="0">
+    <comment ref="B88" authorId="0">
       <text>
         <t>ObjectID:F516FBA4-EF01-065E-D1BD-B89E419DA854;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B61" authorId="0">
+    <comment ref="B89" authorId="0">
       <text>
         <t>ObjectID:FD482B8E-FAC4-14B8-B6F7-4BB4493553D6;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B62" authorId="0">
+    <comment ref="B90" authorId="0">
       <text>
         <t>ObjectID:E0B817CD-92CC-96B2-7333-4216A6F1F009;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B63" authorId="0">
+    <comment ref="B91" authorId="0">
       <text>
         <t>ObjectID:4666453C-838B-2004-8F14-E5FC0FD49A0D;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B64" authorId="0">
+    <comment ref="B92" authorId="0">
       <text>
         <t>ObjectID:885D6A6C-4AA2-2EE3-94EF-A44CE8C47F48;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B65" authorId="0">
+    <comment ref="B93" authorId="0">
       <text>
         <t>ObjectID:10917FDA-EAFE-66E7-E4AE-80E895184321;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B70" authorId="0">
+    <comment ref="B98" authorId="0">
       <text>
         <t>ObjectID:62EBD44D-5232-8674-53C9-D3354174D34D;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <t>ObjectID:AEF47B43-F984-0D17-0267-F3B5CE8756C5;
 Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <t>ObjectID:F0CDA38B-B9FC-DC3D-6BA2-8159C3CD8503;
 Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
       </text>
     </comment>
-    <comment ref="A79" authorId="0">
+    <comment ref="A107" authorId="0">
       <text>
         <t>ObjectID:F2C75C8A-7424-7680-AC53-F0DFE07B3F68;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B111" authorId="0">
       <text>
         <t>ObjectID:DED107D2-07E2-FE6A-19B3-970E7C3D9AC5;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B112" authorId="0">
       <text>
         <t>ObjectID:2CA22C0F-3E70-79E3-4CC1-4D8A18C741B5;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B89" authorId="0">
+    <comment ref="B117" authorId="0">
       <text>
         <t>ObjectID:C4CE16E0-1C34-C60B-F850-1418FF1D438C;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="A92" authorId="0">
+    <comment ref="A120" authorId="0">
       <text>
         <t>ObjectID:4EA60C2F-6DE0-8FCA-8C38-BE4ADEFBDBC8;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B96" authorId="0">
+    <comment ref="B124" authorId="0">
       <text>
         <t>ObjectID:C66B576B-F4C3-B565-CBCC-2F9C07762CEB;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B97" authorId="0">
+    <comment ref="B125" authorId="0">
       <text>
         <t>ObjectID:5A53AED5-921A-1EAC-CF85-5C1022A47953;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B98" authorId="0">
+    <comment ref="B126" authorId="0">
       <text>
         <t>ObjectID:FADC9424-B13F-6201-4225-C82C31C6B6C7;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B99" authorId="0">
+    <comment ref="B127" authorId="0">
       <text>
         <t>ObjectID:AC31F942-C982-B549-3F8B-C9A5669F7285;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B132" authorId="0">
       <text>
         <t>ObjectID:09070F35-9366-9BDE-093A-87B391F0CC0D;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B133" authorId="0">
       <text>
         <t>ObjectID:65B650A4-1196-466E-D77A-BC26ECFA0C91;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="A108" authorId="0">
+    <comment ref="A136" authorId="0">
       <text>
         <t>ObjectID:AF2AB5F5-1EE8-D50A-F20B-74D099FA9E1B;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B112" authorId="0">
+    <comment ref="B140" authorId="0">
       <text>
         <t>ObjectID:88182613-8C6B-8237-4F2B-E8615A23F3CF;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B113" authorId="0">
+    <comment ref="B141" authorId="0">
       <text>
         <t>ObjectID:525758B3-8BF8-B3F4-269D-7E269B8FB8D6;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B118" authorId="0">
+    <comment ref="B146" authorId="0">
       <text>
         <t>ObjectID:2750E838-82E6-5BA0-1CC6-AF1BCDC7990E;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="A121" authorId="0">
+    <comment ref="A149" authorId="0">
       <text>
         <t>ObjectID:96CFC6A1-ABBE-B422-0E42-6AA357B64458;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B125" authorId="0">
+    <comment ref="B153" authorId="0">
       <text>
         <t>ObjectID:E562EC6C-79B5-BB43-A61E-0BDCE6F58C77;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B126" authorId="0">
+    <comment ref="B154" authorId="0">
       <text>
         <t>ObjectID:22BEF716-1B55-B0BA-1EFD-B33AA7BF463A;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B131" authorId="0">
+    <comment ref="B159" authorId="0">
       <text>
         <t>ObjectID:CA986A16-12BB-6001-C706-D958874031BB;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="A134" authorId="0">
+    <comment ref="A162" authorId="0">
       <text>
         <t>ObjectID:69284A30-8A7E-E4B1-0B3F-68E7D639F73B;
 Class:oracle.dbtools.crest.model.design.relational.Table</t>
       </text>
     </comment>
-    <comment ref="B138" authorId="0">
+    <comment ref="B166" authorId="0">
       <text>
         <t>ObjectID:19F8BCC2-46F4-3860-CEB0-0876A3E8F514;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B139" authorId="0">
+    <comment ref="B167" authorId="0">
       <text>
         <t>ObjectID:E125D840-CC95-E1F5-6789-03C58AA73907;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B140" authorId="0">
+    <comment ref="B168" authorId="0">
       <text>
         <t>ObjectID:0DED2D0A-5259-C377-320D-508BC6692377;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B141" authorId="0">
+    <comment ref="B169" authorId="0">
       <text>
         <t>ObjectID:FC60D487-E0AC-FCB5-5FA7-677B262EFD17;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B142" authorId="0">
+    <comment ref="B170" authorId="0">
       <text>
         <t>ObjectID:A93C9E7C-8CE1-EB9D-D8A4-515D60140F83;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B143" authorId="0">
+    <comment ref="B171" authorId="0">
       <text>
         <t>ObjectID:B44BE613-54E9-ABE6-BF19-9D383A6E1969;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B148" authorId="0">
+    <comment ref="B176" authorId="0">
       <text>
         <t>ObjectID:E989073F-64A2-968B-2476-F9C9A1414F26;
 Class:oracle.dbtools.crest.model.design.relational.Index</t>
       </text>
     </comment>
-    <comment ref="B153" authorId="0">
+    <comment ref="B181" authorId="0">
       <text>
         <t>ObjectID:8717AB4A-5939-A800-7CEA-EF0E6237C048;
 Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
       </text>
     </comment>
-    <comment ref="A156" authorId="0">
-      <text>
-        <t>ObjectID:9EB277BE-7029-BA3A-7ED2-D3038A5BB0F7;
-Class:oracle.dbtools.crest.model.design.relational.Table</t>
-      </text>
-    </comment>
-    <comment ref="B160" authorId="0">
-      <text>
-        <t>ObjectID:0A748269-11F0-6F0A-4667-79981867EE71;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B161" authorId="0">
-      <text>
-        <t>ObjectID:0DC8528D-621E-B3E6-D588-8692D6E45ECE;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B162" authorId="0">
-      <text>
-        <t>ObjectID:BD88747F-A567-E695-8FB1-F158C888E4A5;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B163" authorId="0">
-      <text>
-        <t>ObjectID:C6B9DCF9-EBFB-8590-7CB3-4536F9387A30;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B164" authorId="0">
-      <text>
-        <t>ObjectID:7961CC4F-BA66-2228-A932-0B0346F7A562;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B165" authorId="0">
-      <text>
-        <t>ObjectID:116A239F-1C67-FC1B-6815-35D5ACAE992B;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B166" authorId="0">
-      <text>
-        <t>ObjectID:D4892A06-5DB8-541D-0CE1-87349B9F7CF4;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B167" authorId="0">
-      <text>
-        <t>ObjectID:BFBDF889-A7E4-DCFD-EBC4-7B96A816B970;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B168" authorId="0">
-      <text>
-        <t>ObjectID:1B3869AC-9231-7FC5-BD2B-AF1B3A58E1BC;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B169" authorId="0">
-      <text>
-        <t>ObjectID:506CC65D-B1AB-F31A-4BA9-517671DDF7B6;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B170" authorId="0">
-      <text>
-        <t>ObjectID:EFBBC641-A321-85C6-19C5-7484C997CEB6;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B175" authorId="0">
-      <text>
-        <t>ObjectID:DB34C21D-3EE5-7339-632A-053443C65A1D;
-Class:oracle.dbtools.crest.model.design.relational.Index</t>
-      </text>
-    </comment>
-    <comment ref="B180" authorId="0">
-      <text>
-        <t>ObjectID:5672E553-2046-F443-A1CF-5056EFCC6128;
-Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
-      </text>
-    </comment>
-    <comment ref="B181" authorId="0">
-      <text>
-        <t>ObjectID:E465E2CF-3E8A-BC03-97AD-612D80B1ED1A;
-Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
-      </text>
-    </comment>
     <comment ref="A184" authorId="0">
       <text>
         <t>ObjectID:61405D3B-E3C2-9C1E-3780-7358DAEE4C55;
@@ -482,34 +482,34 @@
     </comment>
     <comment ref="B188" authorId="0">
       <text>
+        <t>ObjectID:132D178D-440C-BDFB-DFC0-9FB51BF534F4;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B189" authorId="0">
+      <text>
+        <t>ObjectID:216F7602-97B8-7D36-33DB-8D81101285F0;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B190" authorId="0">
+      <text>
+        <t>ObjectID:2B383476-AC5D-1802-D02D-FF4D722B6616;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B191" authorId="0">
+      <text>
+        <t>ObjectID:18A15F6C-C5AC-809C-69A3-14404A8C4E90;
+Class:oracle.dbtools.crest.model.design.relational.Column</t>
+      </text>
+    </comment>
+    <comment ref="B192" authorId="0">
+      <text>
         <t>ObjectID:02FCF6E1-B6F1-B982-748D-28A7D8CC1F28;
 Class:oracle.dbtools.crest.model.design.relational.Column</t>
       </text>
     </comment>
-    <comment ref="B189" authorId="0">
-      <text>
-        <t>ObjectID:132D178D-440C-BDFB-DFC0-9FB51BF534F4;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B190" authorId="0">
-      <text>
-        <t>ObjectID:216F7602-97B8-7D36-33DB-8D81101285F0;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B191" authorId="0">
-      <text>
-        <t>ObjectID:2B383476-AC5D-1802-D02D-FF4D722B6616;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
-    <comment ref="B192" authorId="0">
-      <text>
-        <t>ObjectID:18A15F6C-C5AC-809C-69A3-14404A8C4E90;
-Class:oracle.dbtools.crest.model.design.relational.Column</t>
-      </text>
-    </comment>
     <comment ref="B193" authorId="0">
       <text>
         <t>ObjectID:4D95F55A-C97C-3C3B-8327-6B534B5E9C7C;
@@ -536,13 +536,13 @@
     </comment>
     <comment ref="B205" authorId="0">
       <text>
+        <t>ObjectID:BD842AAB-E5CA-2B05-3971-96A4C81CA41C;
+Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
+      </text>
+    </comment>
+    <comment ref="B206" authorId="0">
+      <text>
         <t>ObjectID:08041685-0A79-C282-89D5-F8E79385DDB1;
-Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
-      </text>
-    </comment>
-    <comment ref="B206" authorId="0">
-      <text>
-        <t>ObjectID:BD842AAB-E5CA-2B05-3971-96A4C81CA41C;
 Class:oracle.dbtools.crest.model.design.relational.FKIndexAssociation</t>
       </text>
     </comment>
@@ -637,6 +637,12 @@
     <t>Address</t>
   </si>
   <si>
+    <t>9EB277BE-7029-BA3A-7ED2-D3038A5BB0F7</t>
+  </si>
+  <si>
+    <t>AppUser</t>
+  </si>
+  <si>
     <t>18144285-2A12-39D4-D8F8-0A3A21C806E9</t>
   </si>
   <si>
@@ -685,12 +691,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>9EB277BE-7029-BA3A-7ED2-D3038A5BB0F7</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>61405D3B-E3C2-9C1E-3780-7358DAEE4C55</t>
   </si>
   <si>
@@ -796,6 +796,12 @@
     <t>idAddress</t>
   </si>
   <si>
+    <t>02FCF6E1-B6F1-B982-748D-28A7D8CC1F28</t>
+  </si>
+  <si>
+    <t>idAppUser</t>
+  </si>
+  <si>
     <t>E0B817CD-92CC-96B2-7333-4216A6F1F009</t>
   </si>
   <si>
@@ -946,12 +952,6 @@
     <t>streetNumber</t>
   </si>
   <si>
-    <t>02FCF6E1-B6F1-B982-748D-28A7D8CC1F28</t>
-  </si>
-  <si>
-    <t>User_idUser</t>
-  </si>
-  <si>
     <t>10917FDA-EAFE-66E7-E4AE-80E895184321</t>
   </si>
   <si>
@@ -1006,24 +1006,30 @@
     <t>User_Contract_FK</t>
   </si>
   <si>
+    <t>BD842AAB-E5CA-2B05-3971-96A4C81CA41C</t>
+  </si>
+  <si>
+    <t>UserDevice_AppUser_FK</t>
+  </si>
+  <si>
     <t>08041685-0A79-C282-89D5-F8E79385DDB1</t>
   </si>
   <si>
     <t>UserDevice_Device_FK</t>
   </si>
   <si>
-    <t>BD842AAB-E5CA-2B05-3971-96A4C81CA41C</t>
-  </si>
-  <si>
-    <t>UserDevice_User_FK</t>
-  </si>
-  <si>
     <t>2B5755DD-BFDB-0AB3-056A-013C56E9B981</t>
   </si>
   <si>
     <t>Address_PK</t>
   </si>
   <si>
+    <t>DB34C21D-3EE5-7339-632A-053443C65A1D</t>
+  </si>
+  <si>
+    <t>AppUser_PK</t>
+  </si>
+  <si>
     <t>A3A2543F-CEE5-46DD-9744-09F43056D2BD</t>
   </si>
   <si>
@@ -1072,12 +1078,6 @@
     <t>Result_PK</t>
   </si>
   <si>
-    <t>DB34C21D-3EE5-7339-632A-053443C65A1D</t>
-  </si>
-  <si>
-    <t>User_PK</t>
-  </si>
-  <si>
     <t>DA77D18B-BFD6-B633-60E9-7CDE685E7A68</t>
   </si>
   <si>
@@ -1607,6 +1607,27 @@
   </si>
   <si>
     <t xml:space="preserve">Generate in DDL </t>
+  </si>
+  <si>
+    <t>VARCHAR2 (3)</t>
+  </si>
+  <si>
+    <t>VARCHAR2 (500)</t>
+  </si>
+  <si>
+    <t>VARCHAR2 (20)</t>
+  </si>
+  <si>
+    <t>VARCHAR2 (12)</t>
+  </si>
+  <si>
+    <t>NUMBER (9)</t>
+  </si>
+  <si>
+    <t>RAW (255)</t>
+  </si>
+  <si>
+    <t>AppUser.id</t>
   </si>
   <si>
     <t>NUMBER (2)</t>
@@ -1627,9 +1648,6 @@
     <t>ChargeType.id</t>
   </si>
   <si>
-    <t>VARCHAR2 (20)</t>
-  </si>
-  <si>
     <t>Comuna.id</t>
   </si>
   <si>
@@ -1672,9 +1690,6 @@
     <t>Contiene mediciones de dispositivo despues de los 60 minutos</t>
   </si>
   <si>
-    <t>NUMBER (9)</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -1682,21 +1697,6 @@
   </si>
   <si>
     <t>Result.id</t>
-  </si>
-  <si>
-    <t>VARCHAR2 (3)</t>
-  </si>
-  <si>
-    <t>VARCHAR2 (500)</t>
-  </si>
-  <si>
-    <t>VARCHAR2 (12)</t>
-  </si>
-  <si>
-    <t>RAW (255)</t>
-  </si>
-  <si>
-    <t>User.id</t>
   </si>
   <si>
     <t>VARCHAR2 (30)</t>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="11" ht="18.0" customHeight="true">
       <c r="B11" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>331</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="12" ht="18.0" customHeight="true">
       <c r="B12" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>331</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="13" ht="18.0" customHeight="true">
       <c r="B13" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>331</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="14" ht="18.0" customHeight="true">
       <c r="B14" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>332</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="15" ht="18.0" customHeight="true">
       <c r="B15" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>331</v>
@@ -2223,10 +2223,10 @@
         <v>136</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>334</v>
@@ -2246,10 +2246,10 @@
         <v>138</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>334</v>
@@ -2269,10 +2269,10 @@
         <v>140</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>334</v>
@@ -2357,16 +2357,16 @@
     </row>
     <row r="34" ht="18.0" customHeight="true">
       <c r="B34" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>352</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>336</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="35" ht="18.0" customHeight="true">
       <c r="B35" s="6" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>353</v>
@@ -2398,356 +2398,432 @@
         <v>322</v>
       </c>
       <c r="H35" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="36" ht="18.0" customHeight="true">
+      <c r="B36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>354</v>
       </c>
+      <c r="D36" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="37" ht="18.0" customHeight="true">
+      <c r="B37" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="38" ht="18.0" customHeight="true">
-      <c r="B38" t="s" s="5">
-        <v>339</v>
+      <c r="B38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="39" ht="18.0" customHeight="true">
-      <c r="B39" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>325</v>
+      <c r="B39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="40" ht="18.0" customHeight="true">
       <c r="B40" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C40" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="41" ht="18.0" customHeight="true">
+      <c r="B41" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="42" ht="18.0" customHeight="true">
+      <c r="B42" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="43" ht="18.0" customHeight="true">
+      <c r="B43" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" ht="18.0" customHeight="true">
+      <c r="B44" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="47" ht="18.0" customHeight="true">
+      <c r="B47" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="48" ht="18.0" customHeight="true">
+      <c r="B48" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="49" ht="18.0" customHeight="true">
+      <c r="B49" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="E40" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="42" ht="18.0" customHeight="true">
-      <c r="A42" s="2" t="s">
+      <c r="E49" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" ht="18.0" customHeight="true">
+      <c r="B52" t="s" s="5">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="53" ht="18.0" customHeight="true">
+      <c r="B53" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="54" ht="18.0" customHeight="true">
+      <c r="B54" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="55" ht="18.0" customHeight="true">
+      <c r="B55" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="57" ht="18.0" customHeight="true">
+      <c r="A57" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="43" ht="18.0" customHeight="true">
-      <c r="A43" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B43" s="6" t="s">
+    <row r="58" ht="18.0" customHeight="true">
+      <c r="A58" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="45" ht="18.0" customHeight="true">
-      <c r="B45" t="s" s="5">
+      <c r="C58" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="60" ht="18.0" customHeight="true">
+      <c r="B60" t="s" s="5">
         <v>328</v>
       </c>
     </row>
-    <row r="46" ht="18.0" customHeight="true">
-      <c r="B46" s="3" t="s">
+    <row r="61" ht="18.0" customHeight="true">
+      <c r="B61" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="47" ht="18.0" customHeight="true">
-      <c r="B47" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="48" ht="18.0" customHeight="true">
-      <c r="B48" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="51" ht="18.0" customHeight="true">
-      <c r="B51" t="s" s="5">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="52" ht="18.0" customHeight="true">
-      <c r="B52" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="53" ht="18.0" customHeight="true">
-      <c r="B53" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="55" ht="18.0" customHeight="true">
-      <c r="A55" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="56" ht="18.0" customHeight="true">
-      <c r="A56" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="58" ht="18.0" customHeight="true">
-      <c r="B58" t="s" s="5">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="59" ht="18.0" customHeight="true">
-      <c r="B59" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="60" ht="18.0" customHeight="true">
-      <c r="B60" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="61" ht="18.0" customHeight="true">
-      <c r="B61" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="62" ht="18.0" customHeight="true">
       <c r="B62" s="6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>334</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>322</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63" ht="18.0" customHeight="true">
       <c r="B63" s="6" t="s">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>331</v>
+        <v>360</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>334</v>
@@ -2756,109 +2832,103 @@
         <v>336</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>322</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="64" ht="18.0" customHeight="true">
-      <c r="B64" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="65" ht="18.0" customHeight="true">
-      <c r="B65" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G65" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H65" s="6" t="s">
         <v>361</v>
       </c>
     </row>
+    <row r="66" ht="18.0" customHeight="true">
+      <c r="B66" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="67" ht="18.0" customHeight="true">
+      <c r="B67" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
     <row r="68" ht="18.0" customHeight="true">
-      <c r="B68" t="s" s="5">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="69" ht="18.0" customHeight="true">
-      <c r="B69" s="3" t="s">
+      <c r="B68" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="70" ht="18.0" customHeight="true">
+      <c r="A70" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G69" s="3" t="s">
+      <c r="C70" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="70" ht="18.0" customHeight="true">
-      <c r="B70" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G70" s="6" t="s">
+      <c r="E70" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="71" ht="18.0" customHeight="true">
+      <c r="A71" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="73" ht="18.0" customHeight="true">
       <c r="B73" t="s" s="5">
-        <v>344</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" ht="18.0" customHeight="true">
@@ -2866,19 +2936,19 @@
         <v>323</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>325</v>
@@ -2886,22 +2956,22 @@
     </row>
     <row r="75" ht="18.0" customHeight="true">
       <c r="B75" s="6" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>336</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>322</v>
@@ -2909,650 +2979,659 @@
     </row>
     <row r="76" ht="18.0" customHeight="true">
       <c r="B76" s="6" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>334</v>
+        <v>354</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>336</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="78" ht="18.0" customHeight="true">
-      <c r="A78" s="2" t="s">
+    <row r="79" ht="18.0" customHeight="true">
+      <c r="B79" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="80" ht="18.0" customHeight="true">
+      <c r="B80" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C80" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D80" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="81" ht="18.0" customHeight="true">
+      <c r="B81" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="83" ht="18.0" customHeight="true">
+      <c r="A83" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="79" ht="18.0" customHeight="true">
-      <c r="A79" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B79" s="6" t="s">
+    <row r="84" ht="18.0" customHeight="true">
+      <c r="A84" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="81" ht="18.0" customHeight="true">
-      <c r="B81" t="s" s="5">
+      <c r="C84" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" ht="18.0" customHeight="true">
+      <c r="B86" t="s" s="5">
         <v>328</v>
       </c>
     </row>
-    <row r="82" ht="18.0" customHeight="true">
-      <c r="B82" s="3" t="s">
+    <row r="87" ht="18.0" customHeight="true">
+      <c r="B87" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D87" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E87" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="F87" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H87" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="83" ht="18.0" customHeight="true">
-      <c r="B83" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" s="8" t="s">
+    <row r="88" ht="18.0" customHeight="true">
+      <c r="B88" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="D83" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="84" ht="18.0" customHeight="true">
-      <c r="B84" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="87" ht="18.0" customHeight="true">
-      <c r="B87" t="s" s="5">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="88" ht="18.0" customHeight="true">
-      <c r="B88" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>325</v>
+      <c r="D88" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="89" ht="18.0" customHeight="true">
       <c r="B89" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>341</v>
+        <v>68</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>322</v>
+        <v>334</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="90" ht="18.0" customHeight="true">
+      <c r="B90" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="91" ht="18.0" customHeight="true">
-      <c r="A91" s="2" t="s">
+      <c r="B91" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="92" ht="18.0" customHeight="true">
+      <c r="B92" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="93" ht="18.0" customHeight="true">
+      <c r="B93" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="96" ht="18.0" customHeight="true">
+      <c r="B96" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="97" ht="18.0" customHeight="true">
+      <c r="B97" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C97" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D91" s="2" t="s">
+      <c r="D97" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G97" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="92" ht="18.0" customHeight="true">
-      <c r="A92" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="94" ht="18.0" customHeight="true">
-      <c r="B94" t="s" s="5">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="95" ht="18.0" customHeight="true">
-      <c r="B95" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="96" ht="18.0" customHeight="true">
-      <c r="B96" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F96" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H96" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="97" ht="18.0" customHeight="true">
-      <c r="B97" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F97" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H97" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="98" ht="18.0" customHeight="true">
       <c r="B98" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>334</v>
+        <v>322</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>341</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H98" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="99" ht="18.0" customHeight="true">
-      <c r="B99" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G99" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H99" s="6" t="s">
-        <v>322</v>
+        <v>368</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="101" ht="18.0" customHeight="true">
+      <c r="B101" t="s" s="5">
+        <v>344</v>
       </c>
     </row>
     <row r="102" ht="18.0" customHeight="true">
-      <c r="B102" t="s" s="5">
-        <v>339</v>
+      <c r="B102" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="103" ht="18.0" customHeight="true">
-      <c r="B103" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>325</v>
+      <c r="B103" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="104" ht="18.0" customHeight="true">
       <c r="B104" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>166</v>
+        <v>144</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="105" ht="18.0" customHeight="true">
-      <c r="B105" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>322</v>
+        <v>170</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="106" ht="18.0" customHeight="true">
+      <c r="A106" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="107" ht="18.0" customHeight="true">
-      <c r="A107" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B107" s="2" t="s">
+      <c r="A107" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="109" ht="18.0" customHeight="true">
+      <c r="B109" t="s" s="5">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="110" ht="18.0" customHeight="true">
+      <c r="B110" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D107" s="2" t="s">
+      <c r="C110" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="H110" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="108" ht="18.0" customHeight="true">
-      <c r="A108" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="110" ht="18.0" customHeight="true">
-      <c r="B110" t="s" s="5">
-        <v>328</v>
-      </c>
     </row>
     <row r="111" ht="18.0" customHeight="true">
-      <c r="B111" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H111" s="3" t="s">
-        <v>325</v>
+      <c r="B111" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="112" ht="18.0" customHeight="true">
       <c r="B112" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G112" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="115" ht="18.0" customHeight="true">
+      <c r="B115" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="116" ht="18.0" customHeight="true">
+      <c r="B116" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="117" ht="18.0" customHeight="true">
+      <c r="B117" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="119" ht="18.0" customHeight="true">
+      <c r="A119" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="120" ht="18.0" customHeight="true">
+      <c r="A120" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="122" ht="18.0" customHeight="true">
+      <c r="B122" t="s" s="5">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="123" ht="18.0" customHeight="true">
+      <c r="B123" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="124" ht="18.0" customHeight="true">
+      <c r="B124" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C112" s="8" t="s">
+      <c r="C124" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="D112" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F112" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G112" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H112" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="113" ht="18.0" customHeight="true">
-      <c r="B113" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G113" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H113" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="116" ht="18.0" customHeight="true">
-      <c r="B116" t="s" s="5">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="117" ht="18.0" customHeight="true">
-      <c r="B117" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="118" ht="18.0" customHeight="true">
-      <c r="B118" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G118" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="120" ht="18.0" customHeight="true">
-      <c r="A120" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="121" ht="18.0" customHeight="true">
-      <c r="A121" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F121" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="123" ht="18.0" customHeight="true">
-      <c r="B123" t="s" s="5">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="124" ht="18.0" customHeight="true">
-      <c r="B124" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F124" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>325</v>
+      <c r="D124" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G124" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H124" s="6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="125" ht="18.0" customHeight="true">
       <c r="B125" s="6" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>334</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F125" s="8" t="s">
         <v>336</v>
@@ -3569,7 +3648,7 @@
         <v>3</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>334</v>
@@ -3587,163 +3666,160 @@
         <v>322</v>
       </c>
     </row>
-    <row r="129" ht="18.0" customHeight="true">
-      <c r="B129" t="s" s="5">
+    <row r="127" ht="18.0" customHeight="true">
+      <c r="B127" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G127" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H127" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="130" ht="18.0" customHeight="true">
+      <c r="B130" t="s" s="5">
         <v>339</v>
       </c>
     </row>
-    <row r="130" ht="18.0" customHeight="true">
-      <c r="B130" s="3" t="s">
+    <row r="131" ht="18.0" customHeight="true">
+      <c r="B131" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C131" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D131" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E130" s="3" t="s">
+      <c r="E131" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="F130" s="3" t="s">
+      <c r="F131" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="G130" s="3" t="s">
+      <c r="G131" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="131" ht="18.0" customHeight="true">
-      <c r="B131" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D131" s="6" t="s">
+    <row r="132" ht="18.0" customHeight="true">
+      <c r="B132" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D132" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="E131" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="F131" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G131" s="6" t="s">
+      <c r="E132" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G132" s="6" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="133" ht="18.0" customHeight="true">
-      <c r="A133" s="2" t="s">
+      <c r="B133" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G133" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="135" ht="18.0" customHeight="true">
+      <c r="A135" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B135" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D135" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E133" s="2" t="s">
+      <c r="E135" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="F135" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="134" ht="18.0" customHeight="true">
-      <c r="A134" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C134" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D134" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E134" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="F134" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
     <row r="136" ht="18.0" customHeight="true">
-      <c r="B136" t="s" s="5">
+      <c r="A136" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="138" ht="18.0" customHeight="true">
+      <c r="B138" t="s" s="5">
         <v>328</v>
       </c>
     </row>
-    <row r="137" ht="18.0" customHeight="true">
-      <c r="B137" s="3" t="s">
+    <row r="139" ht="18.0" customHeight="true">
+      <c r="B139" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D139" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E137" s="3" t="s">
+      <c r="E139" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F137" s="3" t="s">
+      <c r="F139" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G137" s="3" t="s">
+      <c r="G139" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H137" s="3" t="s">
+      <c r="H139" s="3" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="138" ht="18.0" customHeight="true">
-      <c r="B138" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C138" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="D138" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E138" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F138" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G138" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H138" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="139" ht="18.0" customHeight="true">
-      <c r="B139" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C139" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="D139" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E139" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F139" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G139" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H139" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="140" ht="18.0" customHeight="true">
@@ -3771,10 +3847,10 @@
     </row>
     <row r="141" ht="18.0" customHeight="true">
       <c r="B141" s="6" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="D141" s="8" t="s">
         <v>334</v>
@@ -3783,7 +3859,7 @@
         <v>336</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G141" s="8" t="s">
         <v>322</v>
@@ -3792,100 +3868,94 @@
         <v>322</v>
       </c>
     </row>
-    <row r="142" ht="18.0" customHeight="true">
-      <c r="B142" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C142" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="D142" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E142" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F142" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G142" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H142" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="143" ht="18.0" customHeight="true">
-      <c r="B143" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="D143" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E143" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F143" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G143" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H143" s="6" t="s">
-        <v>322</v>
+    <row r="144" ht="18.0" customHeight="true">
+      <c r="B144" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="145" ht="18.0" customHeight="true">
+      <c r="B145" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="146" ht="18.0" customHeight="true">
-      <c r="B146" t="s" s="5">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="147" ht="18.0" customHeight="true">
-      <c r="B147" s="3" t="s">
+      <c r="B146" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E146" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G146" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="148" ht="18.0" customHeight="true">
+      <c r="A148" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="B148" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D147" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F147" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G147" s="3" t="s">
+      <c r="C148" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D148" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="148" ht="18.0" customHeight="true">
-      <c r="B148" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D148" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E148" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="F148" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G148" s="6" t="s">
+      <c r="E148" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="149" ht="18.0" customHeight="true">
+      <c r="A149" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F149" s="6" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="151" ht="18.0" customHeight="true">
       <c r="B151" t="s" s="5">
-        <v>344</v>
+        <v>328</v>
       </c>
     </row>
     <row r="152" ht="18.0" customHeight="true">
@@ -3893,19 +3963,19 @@
         <v>323</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>325</v>
@@ -3913,239 +3983,169 @@
     </row>
     <row r="153" ht="18.0" customHeight="true">
       <c r="B153" s="6" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D153" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E153" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="F153" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E153" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F153" s="8" t="s">
+        <v>336</v>
       </c>
       <c r="G153" s="8" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="H153" s="6" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="155" ht="18.0" customHeight="true">
-      <c r="A155" s="2" t="s">
+    <row r="154" ht="18.0" customHeight="true">
+      <c r="B154" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E154" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F154" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G154" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H154" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="157" ht="18.0" customHeight="true">
+      <c r="B157" t="s" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="158" ht="18.0" customHeight="true">
+      <c r="B158" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="C158" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="D158" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="159" ht="18.0" customHeight="true">
+      <c r="B159" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G159" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="161" ht="18.0" customHeight="true">
+      <c r="A161" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C161" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D155" s="2" t="s">
+      <c r="D161" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E155" s="2" t="s">
+      <c r="E161" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F155" s="2" t="s">
+      <c r="F161" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="156" ht="18.0" customHeight="true">
-      <c r="A156" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B156" s="6" t="s">
+    <row r="162" ht="18.0" customHeight="true">
+      <c r="A162" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C156" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E156" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F156" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="158" ht="18.0" customHeight="true">
-      <c r="B158" t="s" s="5">
+      <c r="C162" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="164" ht="18.0" customHeight="true">
+      <c r="B164" t="s" s="5">
         <v>328</v>
       </c>
     </row>
-    <row r="159" ht="18.0" customHeight="true">
-      <c r="B159" s="3" t="s">
+    <row r="165" ht="18.0" customHeight="true">
+      <c r="B165" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C165" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D165" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E165" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F159" s="3" t="s">
+      <c r="F165" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G159" s="3" t="s">
+      <c r="G165" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H159" s="3" t="s">
+      <c r="H165" s="3" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="160" ht="18.0" customHeight="true">
-      <c r="B160" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C160" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="D160" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F160" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G160" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H160" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="161" ht="18.0" customHeight="true">
-      <c r="B161" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F161" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G161" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H161" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="162" ht="18.0" customHeight="true">
-      <c r="B162" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E162" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F162" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G162" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H162" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="163" ht="18.0" customHeight="true">
-      <c r="B163" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D163" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G163" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H163" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="164" ht="18.0" customHeight="true">
-      <c r="B164" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C164" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F164" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="G164" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H164" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="165" ht="18.0" customHeight="true">
-      <c r="B165" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C165" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D165" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E165" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="G165" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H165" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="166" ht="18.0" customHeight="true">
       <c r="B166" s="6" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="D166" s="8" t="s">
         <v>336</v>
@@ -4165,10 +4165,10 @@
     </row>
     <row r="167" ht="18.0" customHeight="true">
       <c r="B167" s="6" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="D167" s="8" t="s">
         <v>336</v>
@@ -4188,16 +4188,16 @@
     </row>
     <row r="168" ht="18.0" customHeight="true">
       <c r="B168" s="6" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F168" s="8" t="s">
         <v>336</v>
@@ -4211,10 +4211,10 @@
     </row>
     <row r="169" ht="18.0" customHeight="true">
       <c r="B169" s="6" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>378</v>
+        <v>331</v>
       </c>
       <c r="D169" s="8" t="s">
         <v>334</v>
@@ -4223,7 +4223,7 @@
         <v>336</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G169" s="8" t="s">
         <v>322</v>
@@ -4234,132 +4234,132 @@
     </row>
     <row r="170" ht="18.0" customHeight="true">
       <c r="B170" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D170" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F170" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G170" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H170" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="171" ht="18.0" customHeight="true">
+      <c r="B171" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C170" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="D170" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="E170" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F170" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="G170" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H170" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="173" ht="18.0" customHeight="true">
-      <c r="B173" t="s" s="5">
+      <c r="C171" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="D171" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E171" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F171" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G171" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H171" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="174" ht="18.0" customHeight="true">
+      <c r="B174" t="s" s="5">
         <v>339</v>
       </c>
     </row>
-    <row r="174" ht="18.0" customHeight="true">
-      <c r="B174" s="3" t="s">
+    <row r="175" ht="18.0" customHeight="true">
+      <c r="B175" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C174" s="3" t="s">
+      <c r="C175" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D174" s="3" t="s">
+      <c r="D175" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E174" s="3" t="s">
+      <c r="E175" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="F174" s="3" t="s">
+      <c r="F175" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="G174" s="3" t="s">
+      <c r="G175" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="175" ht="18.0" customHeight="true">
-      <c r="B175" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C175" s="6" t="s">
+    <row r="176" ht="18.0" customHeight="true">
+      <c r="B176" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C176" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D175" s="6" t="s">
+      <c r="D176" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="E175" s="8" t="s">
+      <c r="E176" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="F175" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G175" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="178" ht="18.0" customHeight="true">
-      <c r="B178" t="s" s="5">
+      <c r="F176" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="179" ht="18.0" customHeight="true">
+      <c r="B179" t="s" s="5">
         <v>344</v>
       </c>
     </row>
-    <row r="179" ht="18.0" customHeight="true">
-      <c r="B179" s="3" t="s">
+    <row r="180" ht="18.0" customHeight="true">
+      <c r="B180" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C179" s="3" t="s">
+      <c r="C180" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="D179" s="3" t="s">
+      <c r="D180" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="E179" s="3" t="s">
+      <c r="E180" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="F179" s="3" t="s">
+      <c r="F180" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G179" s="3" t="s">
+      <c r="G180" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="H179" s="3" t="s">
+      <c r="H180" s="3" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="180" ht="18.0" customHeight="true">
-      <c r="B180" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C180" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D180" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E180" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="F180" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="G180" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="H180" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="181" ht="18.0" customHeight="true">
       <c r="B181" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="E181" s="7" t="s">
         <v>334</v>
@@ -4444,19 +4444,19 @@
     </row>
     <row r="188" ht="18.0" customHeight="true">
       <c r="B188" s="6" t="s">
-        <v>132</v>
+        <v>49</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E188" s="8" t="s">
         <v>336</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G188" s="8" t="s">
         <v>322</v>
@@ -4467,13 +4467,13 @@
     </row>
     <row r="189" ht="18.0" customHeight="true">
       <c r="B189" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>336</v>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="190" ht="18.0" customHeight="true">
       <c r="B190" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>336</v>
@@ -4513,16 +4513,16 @@
     </row>
     <row r="191" ht="18.0" customHeight="true">
       <c r="B191" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>380</v>
+        <v>331</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E191" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F191" s="8" t="s">
         <v>336</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="192" ht="18.0" customHeight="true">
       <c r="B192" s="6" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C192" s="8" t="s">
         <v>331</v>
@@ -4545,10 +4545,10 @@
         <v>334</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G192" s="8" t="s">
         <v>322</v>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="193" ht="18.0" customHeight="true">
       <c r="B193" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C193" s="8" t="s">
         <v>331</v>
@@ -4582,10 +4582,10 @@
     </row>
     <row r="194" ht="18.0" customHeight="true">
       <c r="B194" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="D194" s="8" t="s">
         <v>334</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="195" ht="18.0" customHeight="true">
       <c r="B195" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C195" s="8" t="s">
         <v>381</v>
@@ -4704,10 +4704,10 @@
         <v>152</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E205" s="7" t="s">
         <v>334</v>
@@ -4727,10 +4727,10 @@
         <v>154</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E206" s="7" t="s">
         <v>334</v>
@@ -4787,100 +4787,100 @@
     <dataValidation type="list" sqref="A30" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B40" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B49" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A43" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="D54" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>lov_4!B1:B65000</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="D55" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>lov_4!B1:B65000</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="E54" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="E55" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="F54" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="F55" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="A58" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B53" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B68" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A56" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A71" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B70" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B81" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="D75" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A84" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>null!B1:B65000</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B98" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+      <formula1>null!B1:B65000</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="D103" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>lov_4!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="D76" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="D104" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>lov_4!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="E75" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="E103" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="E76" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="E104" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="F75" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="F103" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="F76" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="F104" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A79" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A107" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B89" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B117" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A92" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A120" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B104" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B132" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B105" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B133" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A108" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A136" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B118" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B146" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A121" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A149" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B131" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B159" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A134" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="A162" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B148" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
+    <dataValidation type="list" sqref="B176" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>null!B1:B65000</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="D153" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>lov_4!B1:B65000</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="E153" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="F153" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="A156" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>null!B1:B65000</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="B175" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>null!B1:B65000</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="D180" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>lov_4!B1:B65000</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="D181" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>lov_4!B1:B65000</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="E180" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
     <dataValidation type="list" sqref="E181" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="F180" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F181" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Entered value is not in valid list of values! _x000a_Choose item from drop down list." showErrorMessage="true">
@@ -5490,12 +5490,12 @@
         <v>109</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>3</v>
@@ -5503,7 +5503,7 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>3</v>
@@ -5511,7 +5511,7 @@
     </row>
     <row r="40">
       <c r="A40" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>3</v>
@@ -5519,7 +5519,7 @@
     </row>
     <row r="41">
       <c r="A41" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>3</v>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="42">
       <c r="A42" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>3</v>
@@ -5535,10 +5535,10 @@
     </row>
     <row r="43">
       <c r="A43" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">

</xml_diff>